<commit_message>
Control de Cambios Registrar Elementos
</commit_message>
<xml_diff>
--- a/blocks/inventarios/gestionElementos/registrarElemento/plantilla/archivo_elementos.xlsx
+++ b/blocks/inventarios/gestionElementos/registrarElemento/plantilla/archivo_elementos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="360" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="504" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datos a Cargar" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,14 +14,13 @@
     <sheet name="Tipo IVA" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Tipo de Póliza" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Marca y Serie " sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Hoja7" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="195">
   <si>
     <t>Nivel Inventarios</t>
   </si>
@@ -47,10 +46,22 @@
     <t>Tipo Póliza</t>
   </si>
   <si>
-    <t>Fecha Inicio Póliza</t>
-  </si>
-  <si>
-    <t>Fecha Final Póliza</t>
+    <t>Año Fecha Inicio Póliza</t>
+  </si>
+  <si>
+    <t>Mes Fecha Inicio Póliza</t>
+  </si>
+  <si>
+    <t>Día Fecha Inicio Póliza</t>
+  </si>
+  <si>
+    <t>Año Fecha Final Póliza</t>
+  </si>
+  <si>
+    <t>Mes Fecha Final Póliza</t>
+  </si>
+  <si>
+    <t>Día Fecha Final Póliza</t>
   </si>
   <si>
     <t>Marca</t>
@@ -65,15 +76,12 @@
     <t>UNIDAD</t>
   </si>
   <si>
-    <t>sony</t>
-  </si>
-  <si>
-    <t>qwe123</t>
-  </si>
-  <si>
     <t>cual</t>
   </si>
   <si>
+    <t>as</t>
+  </si>
+  <si>
     <t>código del nivel inventarios</t>
   </si>
   <si>
@@ -591,7 +599,7 @@
   </si>
   <si>
     <t>- El “Tipo de Póliza” SOLO SE APLICA SI el tipo de bien es DEVOLUTIVO (3) de lo contrario deje la casillas vacías relacionadas con la póliza cuando son tipos de bienes de consumo y consumo controlado.
-- Si aplica  la clase “Tipo de Póliza” : "No aplica", no se diligencia los campos Fecha Inicio Póliza,	Fecha Final Póliza</t>
+- Si aplica  la clase “Tipo de Póliza” : "No aplica", no se diligencia los campos Fecha Inicio Póliza,Fecha Final Póliza</t>
   </si>
   <si>
     <t>De Calidad</t>
@@ -606,17 +614,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
-    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -638,14 +644,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -653,32 +657,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="36"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -800,7 +799,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -852,7 +851,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -961,10 +960,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -978,8 +977,11 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1020408163265"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.4897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.8316326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,14 +1021,26 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1036,15 +1050,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.015306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.4897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.8316326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,22 +1111,34 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>41</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>250000</v>
@@ -1107,31 +1146,45 @@
       <c r="G2" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="H2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K2" s="4" t="n">
         <v>15</v>
       </c>
+      <c r="L2" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="N2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>94</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>500000</v>
@@ -1140,20 +1193,72 @@
         <v>6</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="N3" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1165,7 +1270,7 @@
   </sheetPr>
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -1189,16 +1294,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,13 +1317,13 @@
         <v>102</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F2" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,13 +1337,13 @@
         <v>10201</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="13" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1252,13 +1357,13 @@
         <v>10202</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F4" s="13" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,7 +1377,7 @@
         <v>10203</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,7 +1391,7 @@
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,7 +1405,7 @@
         <v>10301</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,7 +1419,7 @@
         <v>10302</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,7 +1433,7 @@
         <v>10303</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,7 +1447,7 @@
         <v>10304</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,7 +1461,7 @@
         <v>104</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,7 +1475,7 @@
         <v>10401</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,7 +1489,7 @@
         <v>10402</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,7 +1503,7 @@
         <v>10403</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,7 +1517,7 @@
         <v>10404</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,7 +1531,7 @@
         <v>109</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,7 +1545,7 @@
         <v>10901</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,7 +1559,7 @@
         <v>10902</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,7 +1573,7 @@
         <v>110</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,7 +1587,7 @@
         <v>11002</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,7 +1601,7 @@
         <v>111</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,7 +1615,7 @@
         <v>11101</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,7 +1629,7 @@
         <v>11102</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,7 +1643,7 @@
         <v>112</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,7 +1657,7 @@
         <v>11201</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,7 +1671,7 @@
         <v>11202</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,7 +1685,7 @@
         <v>11203</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,7 +1699,7 @@
         <v>11204</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,7 +1713,7 @@
         <v>11205</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,7 +1727,7 @@
         <v>113</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,7 +1741,7 @@
         <v>11301</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +1755,7 @@
         <v>11302</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,7 +1769,7 @@
         <v>114</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1783,7 @@
         <v>11401</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1797,7 @@
         <v>11402</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,7 +1811,7 @@
         <v>11403</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1825,7 @@
         <v>11404</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,7 +1839,7 @@
         <v>11405</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,7 +1853,7 @@
         <v>115</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1867,7 @@
         <v>11501</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,7 +1881,7 @@
         <v>11502</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1895,7 @@
         <v>11503</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,7 +1909,7 @@
         <v>11504</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,7 +1923,7 @@
         <v>11505</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,7 +1937,7 @@
         <v>116</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1951,7 @@
         <v>11601</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +1965,7 @@
         <v>11602</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,7 +1979,7 @@
         <v>117</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,7 +1993,7 @@
         <v>11701</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +2007,7 @@
         <v>11702</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,7 +2021,7 @@
         <v>11703</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +2035,7 @@
         <v>11704</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +2049,7 @@
         <v>121</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,7 +2063,7 @@
         <v>125</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,7 +2077,7 @@
         <v>12501</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,7 +2091,7 @@
         <v>12502</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,7 +2105,7 @@
         <v>12503</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,7 +2119,7 @@
         <v>12601</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,7 +2133,7 @@
         <v>12602</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,7 +2161,7 @@
         <v>201</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2175,7 @@
         <v>20101</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,7 +2189,7 @@
         <v>20102</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2098,7 +2203,7 @@
         <v>202</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,7 +2217,7 @@
         <v>20201</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2126,7 +2231,7 @@
         <v>20202</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,7 +2245,7 @@
         <v>20203</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,7 +2259,7 @@
         <v>20204</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,7 +2273,7 @@
         <v>20205</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,7 +2287,7 @@
         <v>20206</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2301,7 @@
         <v>20207</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2210,7 +2315,7 @@
         <v>203</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,7 +2329,7 @@
         <v>20301</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2238,7 +2343,7 @@
         <v>20302</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2252,7 +2357,7 @@
         <v>20303</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,7 +2371,7 @@
         <v>204</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,7 +2385,7 @@
         <v>20401</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2294,7 +2399,7 @@
         <v>20402</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,7 +2413,7 @@
         <v>20403</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2427,7 @@
         <v>20404</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2336,7 +2441,7 @@
         <v>206</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,7 +2455,7 @@
         <v>20601</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,7 +2469,7 @@
         <v>207</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,7 +2483,7 @@
         <v>20701</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,7 +2497,7 @@
         <v>20703</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2406,7 +2511,7 @@
         <v>20704</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,7 +2525,7 @@
         <v>20705</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,7 +2539,7 @@
         <v>20790</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,7 +2553,7 @@
         <v>208</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,7 +2567,7 @@
         <v>20801</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,7 +2581,7 @@
         <v>20802</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,7 +2595,7 @@
         <v>20802</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,7 +2609,7 @@
         <v>209</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,7 +2623,7 @@
         <v>20901</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,7 +2637,7 @@
         <v>20902</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,7 +2651,7 @@
         <v>210</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,7 +2665,7 @@
         <v>21001</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2574,7 +2679,7 @@
         <v>21002</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2588,7 +2693,7 @@
         <v>211</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2602,7 +2707,7 @@
         <v>21101</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2721,7 @@
         <v>21102</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,7 +2735,7 @@
         <v>21108</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2644,7 +2749,7 @@
         <v>212</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,7 +2763,7 @@
         <v>21201</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,7 +2777,7 @@
         <v>21202</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2686,7 +2791,7 @@
         <v>21203</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,7 +2805,7 @@
         <v>213</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,7 +2819,7 @@
         <v>21301</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,7 +2833,7 @@
         <v>21302</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2847,7 @@
         <v>21303</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,7 +2861,7 @@
         <v>214</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,7 +2875,7 @@
         <v>21401</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,7 +2889,7 @@
         <v>21402</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,7 +2903,7 @@
         <v>21403</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2812,7 +2917,7 @@
         <v>21404</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,7 +2931,7 @@
         <v>215</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,7 +2945,7 @@
         <v>21501</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,7 +2959,7 @@
         <v>21502</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2868,7 +2973,7 @@
         <v>21503</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2882,7 +2987,7 @@
         <v>21504</v>
       </c>
       <c r="D120" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,7 +3001,7 @@
         <v>216</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2910,7 +3015,7 @@
         <v>21601</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +3029,7 @@
         <v>21602</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,7 +3043,7 @@
         <v>21603</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2952,7 +3057,7 @@
         <v>21604</v>
       </c>
       <c r="D125" s="12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,7 +3071,7 @@
         <v>218</v>
       </c>
       <c r="D126" s="12" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2980,7 +3085,7 @@
         <v>21801</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2994,7 +3099,7 @@
         <v>220</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,7 +3113,7 @@
         <v>22001</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,7 +3127,7 @@
         <v>22002</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3036,7 +3141,7 @@
         <v>22003</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3050,7 +3155,7 @@
         <v>221</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,7 +3169,7 @@
         <v>22101</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,7 +3183,7 @@
         <v>22102</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,7 +3197,7 @@
         <v>225</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,7 +3211,7 @@
         <v>22501</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,7 +3225,7 @@
         <v>22502</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3134,7 +3239,7 @@
         <v>22503</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,7 +3253,7 @@
         <v>22504</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3162,7 +3267,7 @@
         <v>22505</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,7 +3281,7 @@
         <v>22506</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3190,7 +3295,7 @@
         <v>230</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,7 +3309,7 @@
         <v>3</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,7 +3323,7 @@
         <v>301</v>
       </c>
       <c r="D144" s="12" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,7 +3337,7 @@
         <v>30101</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3246,7 +3351,7 @@
         <v>30102</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3260,7 +3365,7 @@
         <v>4</v>
       </c>
       <c r="D147" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3379,7 @@
         <v>401</v>
       </c>
       <c r="D148" s="12" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3288,7 +3393,7 @@
         <v>402</v>
       </c>
       <c r="D149" s="12" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,7 +3407,7 @@
         <v>403</v>
       </c>
       <c r="D150" s="12" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3316,7 +3421,7 @@
         <v>404</v>
       </c>
       <c r="D151" s="12" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,7 +3435,7 @@
         <v>405</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3344,7 +3449,7 @@
         <v>406</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3358,7 +3463,7 @@
         <v>407</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,7 +3477,7 @@
         <v>408</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,7 +3491,7 @@
         <v>409</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,7 +3505,7 @@
         <v>410</v>
       </c>
       <c r="D157" s="12" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,7 +3519,7 @@
         <v>411</v>
       </c>
       <c r="D158" s="12" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3428,7 +3533,7 @@
         <v>412</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,7 +3547,7 @@
         <v>413</v>
       </c>
       <c r="D160" s="12" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,7 +3561,7 @@
         <v>414</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3470,7 +3575,7 @@
         <v>415</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3478,8 +3583,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3507,7 +3612,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3515,7 +3620,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,7 +3628,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3563,8 +3668,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3593,13 +3698,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="43.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -3615,10 +3720,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
@@ -3634,7 +3739,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
@@ -3659,8 +3764,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3686,7 +3791,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="24" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -3694,7 +3799,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="25" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -3711,34 +3816,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>